<commit_message>
Add upper and lower limit and improve readme
</commit_message>
<xml_diff>
--- a/trendLines/04_Visualization.xlsx
+++ b/trendLines/04_Visualization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rb3ir\Desktop\1_TG\2_Repositories\2_TG-Stella-MDO\trendLines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81453BD1-7417-49D7-9431-04FC006B1123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9C8AFA-3D95-4C27-9449-34D8855F7533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2742877E-9AC8-4387-9240-6DDEA050D879}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="309">
   <si>
     <t>Boeing Insitu ScanEagle</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>MaritimeRobotiocs PX-31</t>
-  </si>
-  <si>
-    <t>22780 </t>
   </si>
   <si>
     <t>Airfoil</t>
@@ -969,7 +966,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -1157,7 +1154,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1475,9 +1472,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64334F66-D899-4A15-9691-020EDA2EA994}">
   <dimension ref="A1:AF83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15"/>
@@ -1514,105 +1511,105 @@
   <sheetData>
     <row r="1" spans="1:32" s="26" customFormat="1">
       <c r="A1" s="26" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="J1" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="26" t="s">
+        <v>283</v>
+      </c>
+      <c r="L1" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>286</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>284</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>288</v>
+      </c>
+      <c r="V1" s="26" t="s">
+        <v>289</v>
+      </c>
+      <c r="W1" s="26" t="s">
+        <v>292</v>
+      </c>
+      <c r="X1" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y1" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="Z1" s="26" t="s">
+        <v>293</v>
+      </c>
+      <c r="AA1" s="26" t="s">
+        <v>281</v>
+      </c>
+      <c r="AB1" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC1" s="26" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="26" t="s">
-        <v>284</v>
-      </c>
-      <c r="L1" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>306</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>307</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>281</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>287</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>285</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>289</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="W1" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="X1" s="27" t="s">
-        <v>302</v>
-      </c>
-      <c r="Y1" s="26" t="s">
-        <v>297</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>294</v>
-      </c>
-      <c r="AA1" s="26" t="s">
+      <c r="AD1" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="AE1" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="AF1" s="26" t="s">
         <v>282</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>278</v>
-      </c>
-      <c r="AD1" s="26" t="s">
-        <v>279</v>
-      </c>
-      <c r="AE1" s="26" t="s">
-        <v>280</v>
-      </c>
-      <c r="AF1" s="26" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="1">
         <v>150</v>
@@ -1638,7 +1635,7 @@
         <v>4500</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N2" s="1">
         <v>7</v>
@@ -1647,22 +1644,22 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AC2" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="AE2" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:32">
@@ -1698,7 +1695,7 @@
         <v>4500</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N3" s="1">
         <v>15.3</v>
@@ -1707,24 +1704,24 @@
         <v>0.2</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AC3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AD3" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="AD3" s="4" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="A4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
@@ -1748,12 +1745,12 @@
         <v>3500</v>
       </c>
       <c r="AC4" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="A5" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1">
         <v>40</v>
@@ -1783,24 +1780,24 @@
         <v>3000</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AC5" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="AD5" s="4" t="s">
         <v>266</v>
-      </c>
-      <c r="AD5" s="4" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>30</v>
@@ -1824,21 +1821,21 @@
         <v>5486</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC6" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD6" s="5" t="s">
         <v>177</v>
-      </c>
-      <c r="AD6" s="5" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:32">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1">
         <v>230</v>
@@ -1862,21 +1859,21 @@
         <v>12</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AC7" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:32">
       <c r="A8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1">
         <v>22</v>
@@ -1906,21 +1903,21 @@
         <v>1.85</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AC8" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:32">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1">
         <v>2.7</v>
@@ -1950,7 +1947,7 @@
         <v>150</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="N9" s="1">
         <v>3.7</v>
@@ -1959,24 +1956,24 @@
         <v>0.3</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="AC9" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD9" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="AD9" s="5" t="s">
+      <c r="AE9" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="AE9" s="6" t="s">
-        <v>186</v>
-      </c>
       <c r="AF9" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:32">
       <c r="A10" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="1">
         <v>6.8</v>
@@ -2004,7 +2001,7 @@
         <v>150</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N10" s="1">
         <v>7.4</v>
@@ -2013,21 +2010,21 @@
         <v>0.38</v>
       </c>
       <c r="AC10" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD10" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="AD10" s="5" t="s">
+      <c r="AE10" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AE10" s="5" t="s">
+      <c r="AF10" s="5" t="s">
         <v>170</v>
-      </c>
-      <c r="AF10" s="5" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:32">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1">
         <v>1.3</v>
@@ -2054,12 +2051,12 @@
         <v>152</v>
       </c>
       <c r="AC11" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="12" spans="1:32">
       <c r="A12" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B12" s="1">
         <v>1.9</v>
@@ -2099,27 +2096,27 @@
         <v>0.22</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC12" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AD12" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="AD12" s="5" t="s">
+      <c r="AE12" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="AE12" s="6" t="s">
+      <c r="AF12" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="AF12" s="6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:32">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="1">
         <v>3.2</v>
@@ -2146,21 +2143,21 @@
         <v>150</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="AC13" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="AD13" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="AD13" s="5" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:32">
       <c r="A14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" s="1">
         <v>570</v>
@@ -2193,12 +2190,12 @@
         <v>3000</v>
       </c>
       <c r="AC14" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:32">
       <c r="A15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1">
         <v>5500</v>
@@ -2225,24 +2222,24 @@
         <v>12000</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AC15" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD15" s="4" t="s">
         <v>236</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:32">
       <c r="A16" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
@@ -2269,18 +2266,18 @@
         <v>1000</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC16" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD16" s="4" t="s">
         <v>240</v>
-      </c>
-      <c r="AD16" s="4" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="17" spans="1:30" s="17" customFormat="1">
       <c r="A17" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B17" s="17">
         <v>650</v>
@@ -2313,10 +2310,10 @@
         <v>5480</v>
       </c>
       <c r="S17" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U17" s="17">
         <v>100</v>
@@ -2325,7 +2322,7 @@
         <v>300</v>
       </c>
       <c r="W17" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X17" s="21">
         <v>5000000</v>
@@ -2334,21 +2331,21 @@
         <v>2014</v>
       </c>
       <c r="Z17" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="AA17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AC17" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AD17" s="19" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1">
         <v>30</v>
@@ -2363,7 +2360,7 @@
         <v>1.5</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G18" s="1">
         <v>41.2</v>
@@ -2381,15 +2378,15 @@
         <v>2700</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AC18" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1">
         <v>17</v>
@@ -2404,7 +2401,7 @@
         <v>1.7</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I19" s="1">
         <v>15</v>
@@ -2416,18 +2413,18 @@
         <v>4000</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AC19" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1">
         <v>9.5</v>
@@ -2457,24 +2454,24 @@
         <v>1000</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AC20" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="AD20" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="AD20" s="4" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1">
         <v>32</v>
@@ -2507,10 +2504,10 @@
         <v>900</v>
       </c>
       <c r="AC21" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="AD21" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="AD21" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:30">
@@ -2546,13 +2543,13 @@
         <v>5900</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AC22" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD22" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="AD22" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:30">
@@ -2584,7 +2581,7 @@
         <v>5950</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N23" s="1">
         <v>12.4</v>
@@ -2593,24 +2590,24 @@
         <v>0.25</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AC23" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="AD23" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="AD23" s="4" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1">
         <v>4.5</v>
@@ -2637,18 +2634,18 @@
         <v>5000</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC24" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="1">
         <v>2.7</v>
@@ -2675,18 +2672,18 @@
         <v>5000</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC25" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:30" s="17" customFormat="1">
       <c r="A26" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B26" s="17">
         <v>1100</v>
@@ -2713,16 +2710,16 @@
         <v>5000</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T26" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U26" s="17">
         <v>100</v>
       </c>
       <c r="W26" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X26" s="21">
         <v>1000000</v>
@@ -2731,18 +2728,18 @@
         <v>2011</v>
       </c>
       <c r="Z26" s="17" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="AA26" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="AC26" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>200</v>
@@ -2772,7 +2769,7 @@
         <v>3600</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="N27" s="1">
         <v>8.23</v>
@@ -2781,24 +2778,24 @@
         <v>0.6</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC27" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AD27" s="5" t="s">
         <v>219</v>
-      </c>
-      <c r="AD27" s="5" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1">
         <v>2.1</v>
@@ -2810,7 +2807,7 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I28" s="1">
         <v>15</v>
@@ -2822,27 +2819,27 @@
         <v>4000</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AC28" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="AD28" s="5" t="s">
         <v>217</v>
-      </c>
-      <c r="AD28" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="29" spans="1:30">
       <c r="A29" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="1">
         <v>15</v>
@@ -2866,12 +2863,12 @@
         <v>3000</v>
       </c>
       <c r="AC29" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1">
         <v>1.5</v>
@@ -2892,21 +2889,21 @@
         <v>6000</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA30" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC30" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="AD30" s="6" t="s">
         <v>255</v>
-      </c>
-      <c r="AD30" s="6" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="1">
         <v>275</v>
@@ -2921,7 +2918,7 @@
         <v>4.63</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G31" s="1">
         <v>51.4</v>
@@ -2936,21 +2933,21 @@
         <v>3600</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA31" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AC31" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1">
         <v>0.69</v>
@@ -2959,7 +2956,7 @@
         <v>0.96</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I32" s="1">
         <v>33</v>
@@ -2968,12 +2965,12 @@
         <v>0.83</v>
       </c>
       <c r="AC32" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:32" s="17" customFormat="1">
       <c r="A33" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="17">
         <v>1180</v>
@@ -3012,16 +3009,16 @@
         <v>0.93700000000000006</v>
       </c>
       <c r="S33" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T33" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U33" s="17">
         <v>115</v>
       </c>
       <c r="W33" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X33" s="21">
         <v>30000000</v>
@@ -3030,27 +3027,27 @@
         <v>2012</v>
       </c>
       <c r="Z33" s="17" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA33" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC33" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD33" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="AE33" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF33" s="17" t="s">
         <v>299</v>
-      </c>
-      <c r="AA33" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC33" s="19" t="s">
-        <v>211</v>
-      </c>
-      <c r="AD33" s="19" t="s">
-        <v>212</v>
-      </c>
-      <c r="AE33" s="19" t="s">
-        <v>213</v>
-      </c>
-      <c r="AF33" s="17" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="28.5" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1">
         <v>4</v>
@@ -3086,24 +3083,24 @@
         <v>0.18</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA34" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC34" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD34" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="AD34" s="6" t="s">
-        <v>183</v>
-      </c>
       <c r="AE34" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:32">
       <c r="A35" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1">
         <v>40</v>
@@ -3127,21 +3124,21 @@
         <v>5000</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA35" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC35" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:32" s="17" customFormat="1">
       <c r="A36" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B36" s="17">
         <v>1633</v>
@@ -3171,16 +3168,16 @@
         <v>8900</v>
       </c>
       <c r="S36" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T36" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U36" s="17">
         <v>165</v>
       </c>
       <c r="W36" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X36" s="21">
         <v>21500000</v>
@@ -3189,24 +3186,24 @@
         <v>2009</v>
       </c>
       <c r="Z36" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AA36" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC36" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD36" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="AD36" s="19" t="s">
+      <c r="AE36" s="19" t="s">
         <v>250</v>
-      </c>
-      <c r="AE36" s="19" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="37" spans="1:32" s="17" customFormat="1">
       <c r="A37" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B37" s="28">
         <v>1020</v>
@@ -3237,7 +3234,7 @@
         <v>7620</v>
       </c>
       <c r="M37" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N37" s="17">
         <v>19</v>
@@ -3249,16 +3246,16 @@
         <v>1.83</v>
       </c>
       <c r="S37" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T37" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U37" s="17">
         <v>115</v>
       </c>
       <c r="W37" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X37" s="21">
         <v>4000000</v>
@@ -3267,24 +3264,24 @@
         <v>1995</v>
       </c>
       <c r="Z37" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AA37" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AC37" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD37" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="AD37" s="19" t="s">
+      <c r="AE37" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="AE37" s="19" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:32" s="17" customFormat="1">
       <c r="A38" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B38" s="17">
         <v>4760</v>
@@ -3314,7 +3311,7 @@
         <v>15000</v>
       </c>
       <c r="M38" s="17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="N38" s="17">
         <v>12</v>
@@ -3323,16 +3320,16 @@
         <v>1.2</v>
       </c>
       <c r="S38" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T38" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U38" s="17">
         <v>900</v>
       </c>
       <c r="W38" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="X38" s="21">
         <v>16900000</v>
@@ -3341,27 +3338,27 @@
         <v>2007</v>
       </c>
       <c r="Z38" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="AA38" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AC38" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="AD38" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="AD38" s="19" t="s">
+      <c r="AE38" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="AE38" s="19" t="s">
+      <c r="AF38" s="19" t="s">
         <v>270</v>
-      </c>
-      <c r="AF38" s="19" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="39" spans="1:32">
       <c r="A39" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" s="1">
         <v>480</v>
@@ -3388,12 +3385,12 @@
         <v>5000</v>
       </c>
       <c r="AC39" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:32">
       <c r="A40" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B40" s="1">
         <v>55</v>
@@ -3417,12 +3414,12 @@
         <v>4572</v>
       </c>
       <c r="AC40" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="1:32">
       <c r="A41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B41" s="1">
         <v>11</v>
@@ -3452,21 +3449,21 @@
         <v>460</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA41" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC41" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AD41" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="AD41" s="4" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:32" s="17" customFormat="1">
       <c r="A42" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B42" s="17">
         <v>450</v>
@@ -3481,7 +3478,7 @@
         <v>5.85</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G42" s="17">
         <v>57</v>
@@ -3496,22 +3493,22 @@
         <v>6400</v>
       </c>
       <c r="M42" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="R42" s="17">
         <v>1.2</v>
       </c>
       <c r="S42" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T42" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U42" s="17">
         <v>47</v>
       </c>
       <c r="W42" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="X42" s="21">
         <v>6000000</v>
@@ -3520,21 +3517,21 @@
         <v>1992</v>
       </c>
       <c r="Z42" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="AA42" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AC42" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AD42" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" spans="1:32">
       <c r="A43" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1">
         <v>27.5</v>
@@ -3561,21 +3558,21 @@
         <v>4500</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T43" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA43" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AC43" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="44" spans="1:32">
       <c r="A44" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B44" s="1">
         <v>125</v>
@@ -3605,24 +3602,24 @@
         <v>1700</v>
       </c>
       <c r="S44" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA44" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AC44" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="AD44" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="AD44" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:32">
       <c r="A45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B45" s="1">
         <v>10</v>
@@ -3634,7 +3631,7 @@
         <v>2</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I45" s="1">
         <v>40</v>
@@ -3646,13 +3643,13 @@
         <v>4600</v>
       </c>
       <c r="AC45" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AD45" s="13"/>
     </row>
     <row r="46" spans="1:32">
       <c r="A46" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B46" s="1">
         <v>2.1</v>
@@ -3682,15 +3679,15 @@
         <v>500</v>
       </c>
       <c r="AA46" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AC46" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:32">
       <c r="A47" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B47" s="1">
         <v>70</v>
@@ -3714,12 +3711,12 @@
         <v>8000</v>
       </c>
       <c r="AC47" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="48" spans="1:32">
       <c r="A48" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="1">
         <v>60</v>
@@ -3749,15 +3746,15 @@
         <v>2000</v>
       </c>
       <c r="AC48" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AD48" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="AD48" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:32">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B49" s="1">
         <v>8.3000000000000007</v>
@@ -3778,18 +3775,18 @@
         <v>5200</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA49" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC49" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:32">
       <c r="A50" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B50" s="1">
         <v>81.8</v>
@@ -3816,12 +3813,12 @@
         <v>4900</v>
       </c>
       <c r="AC50" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:32">
       <c r="A51" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B51" s="1">
         <v>10.9</v>
@@ -3845,16 +3842,16 @@
         <v>3700</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA51" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="AC51" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD51" s="6" t="s">
         <v>246</v>
-      </c>
-      <c r="AD51" s="6" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:32">
@@ -3890,12 +3887,12 @@
         <v>6100</v>
       </c>
       <c r="AC52" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53" spans="1:32">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B53" s="1">
         <v>37.200000000000003</v>
@@ -3925,21 +3922,21 @@
         <v>4500</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T53" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA53" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AC53" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="54" spans="1:32">
       <c r="A54" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="1">
         <v>635</v>
@@ -3966,12 +3963,12 @@
         <v>5500</v>
       </c>
       <c r="AC54" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:32">
       <c r="A55" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="1">
         <v>5.5</v>
@@ -3992,21 +3989,21 @@
         <v>1</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA55" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC55" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AD55" s="4" t="s">
         <v>234</v>
-      </c>
-      <c r="AD55" s="4" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="56" spans="1:32">
       <c r="A56" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B56" s="1">
         <v>159</v>
@@ -4033,21 +4030,21 @@
         <v>5200</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T56" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA56" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AC56" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:32">
       <c r="A57" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B57" s="11">
         <v>14628</v>
@@ -4066,8 +4063,8 @@
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="3" t="s">
-        <v>6</v>
+      <c r="I57" s="3">
+        <v>22780</v>
       </c>
       <c r="J57" s="1">
         <v>32</v>
@@ -4076,36 +4073,36 @@
         <v>18300</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N57" s="1">
         <v>25</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T57" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA57" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC57" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AD57" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="AD57" s="6" t="s">
+      <c r="AE57" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="AE57" s="5" t="s">
+      <c r="AF57" s="5" t="s">
         <v>152</v>
-      </c>
-      <c r="AF57" s="5" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:32">
       <c r="A58" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B58" s="1">
         <v>35</v>
@@ -4138,19 +4135,19 @@
         <v>4000</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T58" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA58" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AC58" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD58" s="4" t="s">
         <v>191</v>
-      </c>
-      <c r="AD58" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="59" spans="1:32">
@@ -4188,18 +4185,18 @@
         <v>30</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA59" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="AC59" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60" spans="1:32">
       <c r="A60" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B60" s="1">
         <v>175</v>
@@ -4226,12 +4223,12 @@
         <v>4500</v>
       </c>
       <c r="AC60" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="61" spans="1:32">
       <c r="A61" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="1">
         <v>5.9</v>
@@ -4258,15 +4255,15 @@
         <v>9100</v>
       </c>
       <c r="AC61" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="AD61" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="AD61" s="5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:32">
       <c r="A62" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62" s="1">
         <v>161</v>
@@ -4296,21 +4293,21 @@
         <v>4000</v>
       </c>
       <c r="S62" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T62" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA62" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AC62" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:32">
       <c r="A63" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B63" s="1">
         <v>20</v>
@@ -4337,18 +4334,18 @@
         <v>8</v>
       </c>
       <c r="S63" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA63" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC63" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="64" spans="1:32">
       <c r="A64" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C64" s="1">
         <v>50</v>
@@ -4372,12 +4369,12 @@
         <v>4572</v>
       </c>
       <c r="AC64" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="65" spans="1:31">
       <c r="A65" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B65" s="1">
         <v>5</v>
@@ -4410,15 +4407,15 @@
         <v>450</v>
       </c>
       <c r="AC65" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD65" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="AD65" s="5" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:31">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="1">
         <v>3.5</v>
@@ -4439,18 +4436,18 @@
         <v>24</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA66" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC66" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" spans="1:31">
       <c r="A67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="1">
         <v>2.8</v>
@@ -4474,18 +4471,18 @@
         <v>450</v>
       </c>
       <c r="S67" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA67" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC67" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="68" spans="1:31">
       <c r="A68" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B68" s="1">
         <v>1600</v>
@@ -4512,24 +4509,24 @@
         <v>9100</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T68" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA68" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AC68" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="AD68" s="6" t="s">
         <v>242</v>
-      </c>
-      <c r="AD68" s="6" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="69" spans="1:31">
       <c r="A69" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B69" s="1">
         <v>4</v>
@@ -4553,12 +4550,12 @@
         <v>2</v>
       </c>
       <c r="AC69" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:31">
       <c r="A70" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B70" s="1">
         <v>180</v>
@@ -4579,12 +4576,12 @@
         <v>20</v>
       </c>
       <c r="AC70" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" spans="1:31">
       <c r="A71" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B71" s="1">
         <v>45.5</v>
@@ -4596,7 +4593,7 @@
         <v>3.7</v>
       </c>
       <c r="F71" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I71" s="1">
         <v>140</v>
@@ -4608,21 +4605,21 @@
         <v>4572</v>
       </c>
       <c r="S71" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T71" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA71" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AC71" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="72" spans="1:31">
       <c r="A72" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B72" s="1">
         <v>20</v>
@@ -4649,12 +4646,12 @@
         <v>3000</v>
       </c>
       <c r="AC72" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:31">
       <c r="A73" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B73" s="1">
         <v>13</v>
@@ -4684,21 +4681,21 @@
         <v>3000</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA73" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AC73" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="AD73" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="AD73" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:31">
       <c r="A74" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B74" s="1">
         <v>40</v>
@@ -4713,7 +4710,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G74" s="1">
         <v>36</v>
@@ -4728,15 +4725,15 @@
         <v>3000</v>
       </c>
       <c r="AC74" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD74" s="5" t="s">
         <v>196</v>
-      </c>
-      <c r="AD74" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:31">
       <c r="A75" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="1">
         <v>2.7</v>
@@ -4757,13 +4754,13 @@
         <v>750</v>
       </c>
       <c r="S75" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA75" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC75" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="76" spans="1:31">
@@ -4805,25 +4802,25 @@
         <v>0.24</v>
       </c>
       <c r="S76" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T76" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA76" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AC76" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD76" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="AD76" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="AE76" s="13"/>
     </row>
     <row r="77" spans="1:31">
       <c r="A77" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B77" s="1">
         <v>3.5</v>
@@ -4844,18 +4841,18 @@
         <v>1.5</v>
       </c>
       <c r="S77" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA77" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC77" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:31">
       <c r="A78" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B78" s="1">
         <v>11</v>
@@ -4882,18 +4879,18 @@
         <v>4000</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA78" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC78" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:31">
       <c r="A79" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B79" s="1">
         <v>85</v>
@@ -4923,21 +4920,21 @@
         <v>5000</v>
       </c>
       <c r="S79" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T79" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA79" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AC79" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:31">
       <c r="A80" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B80" s="1">
         <v>90</v>
@@ -4970,21 +4967,21 @@
         <v>0.52</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T80" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA80" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AC80" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="81" spans="1:29">
       <c r="A81" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B81" s="1">
         <v>105</v>
@@ -5011,7 +5008,7 @@
         <v>3000</v>
       </c>
       <c r="M81" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="N81" s="1">
         <v>12</v>
@@ -5020,21 +5017,21 @@
         <v>0.4</v>
       </c>
       <c r="S81" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T81" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="AA81" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AC81" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="82" spans="1:29" s="17" customFormat="1">
       <c r="A82" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B82" s="17">
         <v>1150</v>
@@ -5067,10 +5064,10 @@
       </c>
       <c r="Q82" s="18"/>
       <c r="S82" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="T82" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U82" s="17">
         <v>115</v>
@@ -5080,12 +5077,12 @@
         <v>2005</v>
       </c>
       <c r="Z82" s="17" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="83" spans="1:29">
       <c r="A83" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B83" s="1">
         <v>3500</v>
@@ -5117,7 +5114,7 @@
         <v>2020</v>
       </c>
       <c r="Z83" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -5470,18 +5467,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5504,6 +5501,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D63523-AED5-4F8F-A4D6-97E385BC0271}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADD8B3EE-C740-4B4E-B8FD-36DEADEC49E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5518,12 +5523,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D2D63523-AED5-4F8F-A4D6-97E385BC0271}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>